<commit_message>
17th September 2014 - Commit#1
</commit_message>
<xml_diff>
--- a/AddRecipe.xlsx
+++ b/AddRecipe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AddRecipe" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>10 Mins</t>
   </si>
@@ -58,16 +58,50 @@
   </si>
   <si>
     <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Pizza</t>
+  </si>
+  <si>
+    <t>Chicken Fajita</t>
+  </si>
+  <si>
+    <t>20 Mins</t>
+  </si>
+  <si>
+    <t>18 mins</t>
+  </si>
+  <si>
+    <t>Cheese</t>
+  </si>
+  <si>
+    <t>250 grams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -90,13 +124,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -426,10 +468,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -449,8 +491,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -461,10 +515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -489,6 +543,23 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -501,10 +572,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -517,6 +588,11 @@
         <v>8</v>
       </c>
     </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -529,9 +605,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -558,8 +636,17 @@
         <v>7</v>
       </c>
     </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
17th September 2014 Commit#2
</commit_message>
<xml_diff>
--- a/AddRecipe.xlsx
+++ b/AddRecipe.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="AddRecipe" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>10 Mins</t>
   </si>
@@ -58,31 +58,13 @@
   </si>
   <si>
     <t>Chocolate</t>
-  </si>
-  <si>
-    <t>Pizza</t>
-  </si>
-  <si>
-    <t>Chicken Fajita</t>
-  </si>
-  <si>
-    <t>20 Mins</t>
-  </si>
-  <si>
-    <t>18 mins</t>
-  </si>
-  <si>
-    <t>Cheese</t>
-  </si>
-  <si>
-    <t>250 grams</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -102,6 +84,12 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -468,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -491,20 +479,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -515,10 +491,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -543,21 +519,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="22.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -570,45 +557,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView showRuler="0" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="1" max="1" width="22.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -636,15 +590,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>